<commit_message>
Uniandes2023: borrador completo programa lenguaje
</commit_message>
<xml_diff>
--- a/Especial_Uniandes_2023/3. Programa de curso/Sesiones curso.xlsx
+++ b/Especial_Uniandes_2023/3. Programa de curso/Sesiones curso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\Especial_Uniandes_2023\3. Programa de curso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7CBDEC-8046-495B-A841-110FACD6DD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF108CD-8DE0-4ECA-A2DE-096ADABB9F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="960" windowWidth="21600" windowHeight="11835" xr2:uid="{79E6B6E8-2283-4874-8159-A333ECA8A106}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{79E6B6E8-2283-4874-8159-A333ECA8A106}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Semana</t>
   </si>
@@ -47,48 +47,9 @@
     <t>Lecturas</t>
   </si>
   <si>
-    <t>16. Evolución de la musicalidad (Fitch, 2005; Leongómez, 2014, Chapter 7)</t>
-  </si>
-  <si>
     <t>Trabajo</t>
   </si>
   <si>
-    <t>(Bee, Perrill, \&amp; Owen, 2000; Charlton \&amp; Reby, 2011; Reby et al., 2005; Ryan, 1980, 1983).</t>
-  </si>
-  <si>
-    <t>(Collins \&amp; Missing, 2003; Collins, 2000; Ferdenzi, Lemaître, Leongómez, \&amp; Roberts, 2011; Puts, Gaulin, \&amp; Verdolini, 2006)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (Hodges-Simeon, Gaulin, \&amp; Puts, 2010; Ohala, 1982; Puts et al., 2006; Puts, Hodges, Cárdenas, \&amp; Gaulin, 2007; Tusing \&amp; Dillard, 2000).</t>
-  </si>
-  <si>
-    <t>(Feinberg et al., 2006; Feinberg, Jones, Little, Burt, \&amp; Perrett, 2005; Leongómez et al., 2014; Pipitone \&amp; Gallup, 2008).</t>
-  </si>
-  <si>
-    <t>(Evans \&amp; Evans, 1999; Greene \&amp; Meagher, 1998; Seyfarth, Cheney, \&amp; Marler, 1980)</t>
-  </si>
-  <si>
-    <t>(Marler \&amp; Pickert, 1984; Podos, Nowicki, \&amp; Peters, 2015)</t>
-  </si>
-  <si>
-    <t>(Dunbar, 1993, 2003; McComb \&amp; Semple, 2005)</t>
-  </si>
-  <si>
-    <t>(Eriksen, Miller, Tougaard, \&amp; Helweg, 2005; Luther \&amp; Baptista, 2010; Noad, Cato, Bryden, Jenner, \&amp; Jenner, 2000)</t>
-  </si>
-  <si>
-    <t>(Fitch, 2000; Hauser, Chomsky, \&amp; Fitch, 2002)</t>
-  </si>
-  <si>
-    <t>(Koelsch, Fritz, Schulze, Alsop, \&amp; Schlaug, 2005; Sammler et al., 2009).</t>
-  </si>
-  <si>
-    <t>(Jentschke, Koelsch, Sallat, \&amp; Friederici, 2008; Pearce, 2005; Signoret, van Eeckhout, Poncet, \&amp; Castaigne, 1987).</t>
-  </si>
-  <si>
-    <t>(Falk, 2005; Kemler Nelson, Hirsh-Pasek, Jusczyk, \&amp; Cassidy, 2009; Papoušek, Papoušek, \&amp; Symmes, 1991)</t>
-  </si>
-  <si>
     <t>Percepción a partir de la voz en animales: tamaño corporal, dominancia, masculinidad-feminidad y selección sexual</t>
   </si>
   <si>
@@ -101,9 +62,6 @@
     <t>Percepción de atractivo físico en humanos: hormonas, masculinidad y feminidad</t>
   </si>
   <si>
-    <t>EXAMEN ¿Qué representa una voz atractiva en humanos?</t>
-  </si>
-  <si>
     <t>Precursores animales del lenguaje: proto-semántica</t>
   </si>
   <si>
@@ -116,9 +74,6 @@
     <t>Discusión general: Ideas sobre el origen del lenguaje</t>
   </si>
   <si>
-    <t>EXAMEN ¿Qué diferencias y similitudes existen entre el lenguaje humano y la comunicación vocal en animales?</t>
-  </si>
-  <si>
     <t>Similitud entre música y lenguaje: evidencia de recursos compartidos</t>
   </si>
   <si>
@@ -131,37 +86,61 @@
     <t>Evolución de la musicalidad</t>
   </si>
   <si>
-    <t>\cite{Collins2000}\linebreak \cite{collinsVocalVisualAttractiveness2003}\linebreak \cite{putsDominanceEvolutionSexual2006}\linebreak \cite{putsSexualSelectionMale2016}\linebreak</t>
-  </si>
-  <si>
-    <t>\cite{evansChickenFoodCalls1999}\linebreak \cite{greeneRedSquirrelsTamiasciurus1998}\linebreak \cite{seyfarthMonkeyResponsesThree1980}\linebreak</t>
-  </si>
-  <si>
-    <t>\cite{marlerSpeciesuniversalMicrostructureLearned1984}\linebreak \cite{podosPermissivenessLearningDevelopment1999}\linebreak</t>
-  </si>
-  <si>
-    <t>\cite{dunbarOriginSubsequentEvolution2003}\linebreak \cite{dunbarCoevolutionNeocorticalSize1993a}\linebreak \cite{mccombCoevolutionVocalCommunication2005}\linebreak</t>
-  </si>
-  <si>
-    <t>\cite{eriksenCulturalChangeSongs2005}\linebreak \cite{lutherUrbanNoiseCultural2010}\linebreak \cite{noadCulturalRevolutionWhale2000}\linebreak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\cite{RefWorks:428}\linebreak </t>
-  </si>
-  <si>
-    <t>\cite{beeMaleGreenFrogs2000}\linebreak \cite{charltonContextrelatedAcousticVariation2011}\linebreak \cite{RefWorks:723}\linebreak</t>
-  </si>
-  <si>
-    <t>\cite{feinbergManipulationsFundamentalFormant2005}\linebreak \cite{RefWorks:385}\linebreak \cite{leongomezVocalModulationCourtship2014}\linebreak</t>
-  </si>
-  <si>
     <t>Evolución cultural de la comunicación vocal: casos animales</t>
   </si>
   <si>
-    <t>\cite{RefWorks:452}\linebreak \cite{leongomezPerceivedDifferencesSocial2017}\linebreak \cite{kleisnerPredictingStrengthAggressive2021}\linebreak \cite{pisanskiReturnOzVoice2014}\linebreak</t>
-  </si>
-  <si>
     <t xml:space="preserve">Introducción y presentación del curso.\linebreak Evolución y significado de las señales vocales. </t>
+  </si>
+  <si>
+    <t>\cite{beeMaleGreenFrogs2000}\linebreak \cite{charltonContextrelatedAcousticVariation2011}\linebreak \cite{RefWorks:723}</t>
+  </si>
+  <si>
+    <t>\cite{RefWorks:452}\linebreak \cite{leongomezPerceivedDifferencesSocial2017}\linebreak \cite{kleisnerPredictingStrengthAggressive2021}\linebreak \cite{pisanskiReturnOzVoice2014}</t>
+  </si>
+  <si>
+    <t>\cite{feinbergManipulationsFundamentalFormant2005}\linebreak \cite{RefWorks:385}\linebreak \cite{leongomezVocalModulationCourtship2014}</t>
+  </si>
+  <si>
+    <t>\cite{evansChickenFoodCalls1999}\linebreak \cite{greeneRedSquirrelsTamiasciurus1998}\linebreak \cite{seyfarthMonkeyResponsesThree1980}</t>
+  </si>
+  <si>
+    <t>\cite{dunbarOriginSubsequentEvolution2003}\linebreak \cite{dunbarCoevolutionNeocorticalSize1993a}\linebreak \cite{mccombCoevolutionVocalCommunication2005}</t>
+  </si>
+  <si>
+    <t>\cite{eriksenCulturalChangeSongs2005}\linebreak \cite{lutherUrbanNoiseCultural2010}\linebreak \cite{noadCulturalRevolutionWhale2000}</t>
+  </si>
+  <si>
+    <t>\cite{jentschkeChildrenSpecificLanguage2008}\linebreak \cite{pearceSelectedObservationsAmusia2005}\linebreak \cite{signoretAphasiaAmusiaBlind1987}</t>
+  </si>
+  <si>
+    <t>\cite{falkPrelinguisticEvolutionEarly2005}\linebreak \cite{kemlernelsonHowProsodicCues2009}\linebreak \cite{papousekMeaningsMelodiesMotherese1991}</t>
+  </si>
+  <si>
+    <t>\cite{RefWorks:428}\linebreak \cite{RefWorks:463}\linebreak \cite{balterEvolutionLanguageAnimal2010}\linebreak \cite{fitchBiologyEvolutionSpeech2018}</t>
+  </si>
+  <si>
+    <t>\cite{fitchBiologyEvolutionMusic2006a}\linebreak \cite{mehrOriginsMusicCredible2021}\linebreak \cite{savageMusicCoevolvedSystem2021}\linebreak \cite{leongomezMusicalityHumanVocal2022}</t>
+  </si>
+  <si>
+    <t>\cite{sammlerOverlapMusicalLinguistic2009}\linebreak \cite{koelschAdultsChildrenProcessing2005}\linebreak \cite{coumelSecondLanguageAccent2019}\linebreak \cite{zuberbuhlerSyntaxCompositionalityAnimal2019}</t>
+  </si>
+  <si>
+    <t>\cite{Collins2000}\linebreak \cite{collinsVocalVisualAttractiveness2003}\linebreak \cite{putsDominanceEvolutionSexual2006}\linebreak \cite{putsSexualSelectionMale2016}</t>
+  </si>
+  <si>
+    <t>\cite{marlerSpeciesuniversalMicrostructureLearned1984}\linebreak \cite{podosPermissivenessLearningDevelopment1999}\linebreak \cite{zuberbuhlerSyntaxCompositionalityAnimal2019}</t>
+  </si>
+  <si>
+    <t>Lectura de artículos\linebreak (Preparación exposición y actividad)</t>
+  </si>
+  <si>
+    <t>ENSAYO ¿Qué diferencias y similitudes existen entre el lenguaje humano y la comunicación vocal en animales?</t>
+  </si>
+  <si>
+    <t>Preparación ensayo</t>
+  </si>
+  <si>
+    <t>ENSAYO ¿Qué señales contiene la voz humana?</t>
   </si>
 </sst>
 </file>
@@ -570,21 +549,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810CEBA7-1363-4AE0-94C3-C2CFA1A440D7}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E18" sqref="E1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="42.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="154.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
+    <col min="3" max="3" width="169.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -595,226 +573,223 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D13" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uniandes 2023: nueva idea sesiones curso lnguaje
</commit_message>
<xml_diff>
--- a/Especial_Uniandes_2023/3. Programa de curso/Sesiones curso.xlsx
+++ b/Especial_Uniandes_2023/3. Programa de curso/Sesiones curso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\Especial_Uniandes_2023\3. Programa de curso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0156F5-25BF-4000-B3FB-2BDF8BD199C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8E9D0F-5123-49FA-8C67-085EB4F84D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{79E6B6E8-2283-4874-8159-A333ECA8A106}"/>
   </bookViews>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810CEBA7-1363-4AE0-94C3-C2CFA1A440D7}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>